<commit_message>
update "export to pdf" lines
</commit_message>
<xml_diff>
--- a/Excel Files/COMP_STATEMENT_CSR.xlsx
+++ b/Excel Files/COMP_STATEMENT_CSR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18195" yWindow="0" windowWidth="33510" windowHeight="20985" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="51480" yWindow="3555" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="STATEMENT" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,11 +18,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="169" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -461,6 +463,26 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="double">
         <color indexed="64"/>
       </top>
@@ -484,26 +506,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -519,7 +521,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -569,6 +571,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -588,13 +591,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -619,8 +622,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,10 +1024,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G49"/>
+  <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
@@ -1067,20 +1072,20 @@
     <row r="7" ht="4.15" customHeight="1"/>
     <row r="8" ht="4.15" customHeight="1" thickBot="1"/>
     <row r="9">
-      <c r="B9" s="27" t="inlineStr">
+      <c r="B9" s="28" t="inlineStr">
         <is>
           <t>Sales Performance</t>
         </is>
       </c>
-      <c r="C9" s="29" t="n"/>
+      <c r="C9" s="30" t="n"/>
       <c r="D9" s="3" t="n"/>
-      <c r="E9" s="27" t="inlineStr">
+      <c r="E9" s="28" t="inlineStr">
         <is>
           <t>Final Payment</t>
         </is>
       </c>
-      <c r="F9" s="28" t="n"/>
-      <c r="G9" s="29" t="n"/>
+      <c r="F9" s="29" t="n"/>
+      <c r="G9" s="30" t="n"/>
     </row>
     <row r="10" ht="16.5" customHeight="1" thickBot="1">
       <c r="B10" s="4" t="inlineStr">
@@ -1092,12 +1097,12 @@
         <f>_xlfn.XLOOKUP("FY_BASE_SALES", payout!$G:$G, payout!$F:$F)</f>
         <v/>
       </c>
-      <c r="E10" s="34" t="inlineStr">
+      <c r="E10" s="35" t="inlineStr">
         <is>
           <t>FY Territory SI Target</t>
         </is>
       </c>
-      <c r="F10" s="35" t="n"/>
+      <c r="F10" s="36" t="n"/>
       <c r="G10" s="19">
         <f>info!B6</f>
         <v/>
@@ -1114,12 +1119,12 @@
         <f>_xlfn.XLOOKUP("YTD_TGT_IMPLANTS", payout!$G:$G, payout!$F:$F)</f>
         <v/>
       </c>
-      <c r="E11" s="41" t="inlineStr">
+      <c r="E11" s="42" t="inlineStr">
         <is>
           <t>FY Territory SI Earned</t>
         </is>
       </c>
-      <c r="F11" s="42" t="n"/>
+      <c r="F11" s="43" t="n"/>
       <c r="G11" s="15">
         <f>(_xlfn.XLOOKUP("YTD_BASE_BONUS_PAID",payout!G:G,payout!F:F))</f>
         <v/>
@@ -1132,27 +1137,27 @@
         </is>
       </c>
       <c r="C12" s="18">
-        <f>IFERROR(G11/G10, 0)</f>
-        <v/>
-      </c>
-      <c r="E12" s="22" t="inlineStr">
+        <f>IFERROR(C10/info!B8, 0)</f>
+        <v/>
+      </c>
+      <c r="E12" s="23" t="inlineStr">
         <is>
           <t>Less Prior Paid</t>
         </is>
       </c>
-      <c r="F12" s="23" t="n"/>
+      <c r="F12" s="24" t="n"/>
       <c r="G12" s="14">
         <f>G11-G13</f>
         <v/>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1" thickTop="1">
-      <c r="E13" s="36" t="inlineStr">
+      <c r="E13" s="37" t="inlineStr">
         <is>
           <t>Territory Payout</t>
         </is>
       </c>
-      <c r="F13" s="37" t="n"/>
+      <c r="F13" s="38" t="n"/>
       <c r="G13" s="13">
         <f>_xlfn.XLOOKUP("BASE_BONUS_PO", payout!G:G,payout!F:F)</f>
         <v/>
@@ -1163,12 +1168,12 @@
         <f>IF(G14&gt;0, 1, 0)</f>
         <v/>
       </c>
-      <c r="E14" s="30" t="inlineStr">
+      <c r="E14" s="33" t="inlineStr">
         <is>
           <t>Target Payout</t>
         </is>
       </c>
-      <c r="F14" s="25" t="n"/>
+      <c r="F14" s="26" t="n"/>
       <c r="G14" s="13">
         <f>IFERROR(_xlfn.XLOOKUP("TGT_BONUS_PO", payout!G:G,payout!F:F), 0)</f>
         <v/>
@@ -1179,24 +1184,24 @@
         <f>IF(G15&gt;0, 1, 0)</f>
         <v/>
       </c>
-      <c r="E15" s="40" t="inlineStr">
+      <c r="E15" s="41" t="inlineStr">
         <is>
           <t>Guarantee Adjustment</t>
         </is>
       </c>
-      <c r="F15" s="25" t="n"/>
+      <c r="F15" s="26" t="n"/>
       <c r="G15" s="5">
         <f>IFERROR(_xlfn.XLOOKUP("GUR_AMT",payout!G:G,payout!F:F), 0)</f>
         <v/>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E16" s="43" t="inlineStr">
+      <c r="E16" s="44" t="inlineStr">
         <is>
           <t>CPAS Payout</t>
         </is>
       </c>
-      <c r="F16" s="35" t="n"/>
+      <c r="F16" s="36" t="n"/>
       <c r="G16" s="7">
         <f>_xlfn.XLOOKUP("CPAS_SPIFF_PO", payout!G:G,payout!F:F)</f>
         <v/>
@@ -1217,598 +1222,578 @@
     <row r="18" ht="4.15" customHeight="1" thickTop="1"/>
     <row r="19" ht="4.15" customHeight="1"/>
     <row r="20">
-      <c r="B20" s="38" t="inlineStr">
+      <c r="B20" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Opportunity Detail </t>
         </is>
       </c>
-      <c r="C20" s="39" t="n"/>
-      <c r="D20" s="39" t="n"/>
-      <c r="E20" s="39" t="n"/>
-      <c r="F20" s="39" t="n"/>
-      <c r="G20" s="25" t="n"/>
+      <c r="C20" s="40" t="n"/>
+      <c r="D20" s="40" t="n"/>
+      <c r="E20" s="40" t="n"/>
+      <c r="F20" s="40" t="n"/>
+      <c r="G20" s="26" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="33" t="inlineStr">
+      <c r="B21" s="34" t="inlineStr">
         <is>
           <t>Account</t>
         </is>
       </c>
-      <c r="C21" s="25" t="n"/>
-      <c r="D21" s="33" t="inlineStr">
+      <c r="C21" s="26" t="n"/>
+      <c r="D21" s="34" t="inlineStr">
         <is>
           <t>Opp Name</t>
         </is>
       </c>
-      <c r="E21" s="25" t="n"/>
-      <c r="F21" s="33" t="inlineStr">
+      <c r="E21" s="26" t="n"/>
+      <c r="F21" s="34" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="G21" s="33" t="inlineStr">
+      <c r="G21" s="34" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="24">
+      <c r="B22" s="25">
         <f>IF(LEN(detail!I2)&lt;1,"",detail!I2)</f>
         <v/>
       </c>
-      <c r="C22" s="25" t="n"/>
-      <c r="D22" s="26">
+      <c r="C22" s="26" t="n"/>
+      <c r="D22" s="27">
         <f>IF(LEN(detail!P2)&lt;1,"",detail!P2) &amp; IF(detail!K2=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E22" s="25" t="n"/>
+      <c r="E22" s="26" t="n"/>
       <c r="F22" s="11">
         <f>IF(LEN(detail!Z2)&lt;1,"",detail!Z2)</f>
         <v/>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="27">
         <f>IF(LEN(detail!W2)&lt;1,"",detail!W2)</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="24">
+      <c r="B23" s="25">
         <f>IF(LEN(detail!I3)&lt;1,"",detail!I3)</f>
         <v/>
       </c>
-      <c r="C23" s="25" t="n"/>
-      <c r="D23" s="26">
+      <c r="C23" s="26" t="n"/>
+      <c r="D23" s="27">
         <f>IF(LEN(detail!P3)&lt;1,"",detail!P3) &amp; IF(detail!K3=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E23" s="25" t="n"/>
+      <c r="E23" s="26" t="n"/>
       <c r="F23" s="11">
         <f>IF(LEN(detail!Z3)&lt;1,"",detail!Z3)</f>
         <v/>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="27">
         <f>IF(LEN(detail!W3)&lt;1,"",detail!W3)</f>
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="24">
+      <c r="B24" s="25">
         <f>IF(LEN(detail!I4)&lt;1,"",detail!I4)</f>
         <v/>
       </c>
-      <c r="C24" s="25" t="n"/>
-      <c r="D24" s="26">
+      <c r="C24" s="26" t="n"/>
+      <c r="D24" s="27">
         <f>IF(LEN(detail!P4)&lt;1,"",detail!P4) &amp; IF(detail!K4=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E24" s="25" t="n"/>
+      <c r="E24" s="26" t="n"/>
       <c r="F24" s="11">
         <f>IF(LEN(detail!Z4)&lt;1,"",detail!Z4)</f>
         <v/>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="27">
         <f>IF(LEN(detail!W4)&lt;1,"",detail!W4)</f>
         <v/>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="24">
+      <c r="B25" s="25">
         <f>IF(LEN(detail!I5)&lt;1,"",detail!I5)</f>
         <v/>
       </c>
-      <c r="C25" s="25" t="n"/>
-      <c r="D25" s="26">
+      <c r="C25" s="26" t="n"/>
+      <c r="D25" s="27">
         <f>IF(LEN(detail!P5)&lt;1,"",detail!P5) &amp; IF(detail!K5=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E25" s="25" t="n"/>
+      <c r="E25" s="26" t="n"/>
       <c r="F25" s="11">
         <f>IF(LEN(detail!Z5)&lt;1,"",detail!Z5)</f>
         <v/>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="27">
         <f>IF(LEN(detail!W5)&lt;1,"",detail!W5)</f>
         <v/>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="24">
+      <c r="B26" s="25">
         <f>IF(LEN(detail!I6)&lt;1,"",detail!I6)</f>
         <v/>
       </c>
-      <c r="C26" s="25" t="n"/>
-      <c r="D26" s="26">
+      <c r="C26" s="26" t="n"/>
+      <c r="D26" s="27">
         <f>IF(LEN(detail!P6)&lt;1,"",detail!P6) &amp; IF(detail!K6=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E26" s="25" t="n"/>
+      <c r="E26" s="26" t="n"/>
       <c r="F26" s="11">
         <f>IF(LEN(detail!Z6)&lt;1,"",detail!Z6)</f>
         <v/>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="27">
         <f>IF(LEN(detail!W6)&lt;1,"",detail!W6)</f>
         <v/>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="24">
+      <c r="B27" s="25">
         <f>IF(LEN(detail!I7)&lt;1,"",detail!I7)</f>
         <v/>
       </c>
-      <c r="C27" s="25" t="n"/>
-      <c r="D27" s="26">
+      <c r="C27" s="26" t="n"/>
+      <c r="D27" s="27">
         <f>IF(LEN(detail!P7)&lt;1,"",detail!P7) &amp; IF(detail!K7=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E27" s="25" t="n"/>
+      <c r="E27" s="26" t="n"/>
       <c r="F27" s="11">
         <f>IF(LEN(detail!Z7)&lt;1,"",detail!Z7)</f>
         <v/>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="27">
         <f>IF(LEN(detail!W7)&lt;1,"",detail!W7)</f>
         <v/>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="24">
+      <c r="B28" s="25">
         <f>IF(LEN(detail!I8)&lt;1,"",detail!I8)</f>
         <v/>
       </c>
-      <c r="C28" s="25" t="n"/>
-      <c r="D28" s="26">
+      <c r="C28" s="26" t="n"/>
+      <c r="D28" s="27">
         <f>IF(LEN(detail!P8)&lt;1,"",detail!P8) &amp; IF(detail!K8=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E28" s="25" t="n"/>
+      <c r="E28" s="26" t="n"/>
       <c r="F28" s="11">
         <f>IF(LEN(detail!Z8)&lt;1,"",detail!Z8)</f>
         <v/>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="27">
         <f>IF(LEN(detail!W8)&lt;1,"",detail!W8)</f>
         <v/>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="24">
+      <c r="B29" s="25">
         <f>IF(LEN(detail!I9)&lt;1,"",detail!I9)</f>
         <v/>
       </c>
-      <c r="C29" s="25" t="n"/>
-      <c r="D29" s="26">
+      <c r="C29" s="26" t="n"/>
+      <c r="D29" s="27">
         <f>IF(LEN(detail!P9)&lt;1,"",detail!P9) &amp; IF(detail!K9=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E29" s="25" t="n"/>
+      <c r="E29" s="26" t="n"/>
       <c r="F29" s="11">
         <f>IF(LEN(detail!Z9)&lt;1,"",detail!Z9)</f>
         <v/>
       </c>
-      <c r="G29" s="26">
+      <c r="G29" s="27">
         <f>IF(LEN(detail!W9)&lt;1,"",detail!W9)</f>
         <v/>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="24">
+      <c r="B30" s="25">
         <f>IF(LEN(detail!I10)&lt;1,"",detail!I10)</f>
         <v/>
       </c>
-      <c r="C30" s="25" t="n"/>
-      <c r="D30" s="26">
+      <c r="C30" s="26" t="n"/>
+      <c r="D30" s="27">
         <f>IF(LEN(detail!P10)&lt;1,"",detail!P10) &amp; IF(detail!K10=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E30" s="25" t="n"/>
+      <c r="E30" s="26" t="n"/>
       <c r="F30" s="11">
         <f>IF(LEN(detail!Z10)&lt;1,"",detail!Z10)</f>
         <v/>
       </c>
-      <c r="G30" s="26">
+      <c r="G30" s="27">
         <f>IF(LEN(detail!W10)&lt;1,"",detail!W10)</f>
         <v/>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="24">
+      <c r="B31" s="25">
         <f>IF(LEN(detail!I11)&lt;1,"",detail!I11)</f>
         <v/>
       </c>
-      <c r="C31" s="25" t="n"/>
-      <c r="D31" s="26">
+      <c r="C31" s="26" t="n"/>
+      <c r="D31" s="27">
         <f>IF(LEN(detail!P11)&lt;1,"",detail!P11) &amp; IF(detail!K11=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E31" s="25" t="n"/>
+      <c r="E31" s="26" t="n"/>
       <c r="F31" s="11">
         <f>IF(LEN(detail!Z11)&lt;1,"",detail!Z11)</f>
         <v/>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="27">
         <f>IF(LEN(detail!W11)&lt;1,"",detail!W11)</f>
         <v/>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="24">
+      <c r="B32" s="25">
         <f>IF(LEN(detail!I12)&lt;1,"",detail!I12)</f>
         <v/>
       </c>
-      <c r="C32" s="25" t="n"/>
-      <c r="D32" s="26">
+      <c r="C32" s="26" t="n"/>
+      <c r="D32" s="27">
         <f>IF(LEN(detail!P12)&lt;1,"",detail!P12) &amp; IF(detail!K12=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E32" s="25" t="n"/>
+      <c r="E32" s="26" t="n"/>
       <c r="F32" s="11">
         <f>IF(LEN(detail!Z12)&lt;1,"",detail!Z12)</f>
         <v/>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="27">
         <f>IF(LEN(detail!W12)&lt;1,"",detail!W12)</f>
         <v/>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="24">
+      <c r="B33" s="25">
         <f>IF(LEN(detail!I13)&lt;1,"",detail!I13)</f>
         <v/>
       </c>
-      <c r="C33" s="25" t="n"/>
-      <c r="D33" s="26">
+      <c r="C33" s="26" t="n"/>
+      <c r="D33" s="27">
         <f>IF(LEN(detail!P13)&lt;1,"",detail!P13) &amp; IF(detail!K13=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E33" s="25" t="n"/>
+      <c r="E33" s="26" t="n"/>
       <c r="F33" s="11">
         <f>IF(LEN(detail!Z13)&lt;1,"",detail!Z13)</f>
         <v/>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="27">
         <f>IF(LEN(detail!W13)&lt;1,"",detail!W13)</f>
         <v/>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="24">
+      <c r="B34" s="25">
         <f>IF(LEN(detail!I14)&lt;1,"",detail!I14)</f>
         <v/>
       </c>
-      <c r="C34" s="25" t="n"/>
-      <c r="D34" s="26">
+      <c r="C34" s="26" t="n"/>
+      <c r="D34" s="27">
         <f>IF(LEN(detail!P14)&lt;1,"",detail!P14) &amp; IF(detail!K14=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E34" s="25" t="n"/>
+      <c r="E34" s="26" t="n"/>
       <c r="F34" s="11">
         <f>IF(LEN(detail!Z14)&lt;1,"",detail!Z14)</f>
         <v/>
       </c>
-      <c r="G34" s="26">
+      <c r="G34" s="27">
         <f>IF(LEN(detail!W14)&lt;1,"",detail!W14)</f>
         <v/>
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="24">
+      <c r="B35" s="25">
         <f>IF(LEN(detail!I15)&lt;1,"",detail!I15)</f>
         <v/>
       </c>
-      <c r="C35" s="25" t="n"/>
-      <c r="D35" s="26">
+      <c r="C35" s="26" t="n"/>
+      <c r="D35" s="27">
         <f>IF(LEN(detail!P15)&lt;1,"",detail!P15) &amp; IF(detail!K15=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E35" s="25" t="n"/>
+      <c r="E35" s="26" t="n"/>
       <c r="F35" s="11">
         <f>IF(LEN(detail!Z15)&lt;1,"",detail!Z15)</f>
         <v/>
       </c>
-      <c r="G35" s="26">
+      <c r="G35" s="27">
         <f>IF(LEN(detail!W15)&lt;1,"",detail!W15)</f>
         <v/>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="24">
+      <c r="B36" s="25">
         <f>IF(LEN(detail!I16)&lt;1,"",detail!I16)</f>
         <v/>
       </c>
-      <c r="C36" s="25" t="n"/>
-      <c r="D36" s="26">
+      <c r="C36" s="26" t="n"/>
+      <c r="D36" s="27">
         <f>IF(LEN(detail!P16)&lt;1,"",detail!P16) &amp; IF(detail!K16=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E36" s="25" t="n"/>
+      <c r="E36" s="26" t="n"/>
       <c r="F36" s="11">
         <f>IF(LEN(detail!Z16)&lt;1,"",detail!Z16)</f>
         <v/>
       </c>
-      <c r="G36" s="26">
+      <c r="G36" s="27">
         <f>IF(LEN(detail!W16)&lt;1,"",detail!W16)</f>
         <v/>
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="24">
+      <c r="B37" s="25">
         <f>IF(LEN(detail!I17)&lt;1,"",detail!I17)</f>
         <v/>
       </c>
-      <c r="C37" s="25" t="n"/>
-      <c r="D37" s="26">
+      <c r="C37" s="26" t="n"/>
+      <c r="D37" s="27">
         <f>IF(LEN(detail!P17)&lt;1,"",detail!P17) &amp; IF(detail!K17=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E37" s="25" t="n"/>
+      <c r="E37" s="26" t="n"/>
       <c r="F37" s="11">
         <f>IF(LEN(detail!Z17)&lt;1,"",detail!Z17)</f>
         <v/>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="27">
         <f>IF(LEN(detail!W17)&lt;1,"",detail!W17)</f>
         <v/>
       </c>
     </row>
     <row r="38">
-      <c r="B38" s="24">
+      <c r="B38" s="25">
         <f>IF(LEN(detail!I18)&lt;1,"",detail!I18)</f>
         <v/>
       </c>
-      <c r="C38" s="25" t="n"/>
-      <c r="D38" s="26">
+      <c r="C38" s="26" t="n"/>
+      <c r="D38" s="27">
         <f>IF(LEN(detail!P18)&lt;1,"",detail!P18) &amp; IF(detail!K18=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E38" s="25" t="n"/>
+      <c r="E38" s="26" t="n"/>
       <c r="F38" s="11">
         <f>IF(LEN(detail!Z18)&lt;1,"",detail!Z18)</f>
         <v/>
       </c>
-      <c r="G38" s="26">
+      <c r="G38" s="27">
         <f>IF(LEN(detail!W18)&lt;1,"",detail!W18)</f>
         <v/>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="24">
+      <c r="B39" s="25">
         <f>IF(LEN(detail!I19)&lt;1,"",detail!I19)</f>
         <v/>
       </c>
-      <c r="C39" s="25" t="n"/>
-      <c r="D39" s="26">
+      <c r="C39" s="26" t="n"/>
+      <c r="D39" s="27">
         <f>IF(LEN(detail!P19)&lt;1,"",detail!P19) &amp; IF(detail!K19=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E39" s="25" t="n"/>
+      <c r="E39" s="26" t="n"/>
       <c r="F39" s="11">
         <f>IF(LEN(detail!Z19)&lt;1,"",detail!Z19)</f>
         <v/>
       </c>
-      <c r="G39" s="26">
+      <c r="G39" s="27">
         <f>IF(LEN(detail!W19)&lt;1,"",detail!W19)</f>
         <v/>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="24">
+      <c r="B40" s="25">
         <f>IF(LEN(detail!I20)&lt;1,"",detail!I20)</f>
         <v/>
       </c>
-      <c r="C40" s="25" t="n"/>
-      <c r="D40" s="26">
+      <c r="C40" s="26" t="n"/>
+      <c r="D40" s="27">
         <f>IF(LEN(detail!P20)&lt;1,"",detail!P20) &amp; IF(detail!K20=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E40" s="25" t="n"/>
+      <c r="E40" s="26" t="n"/>
       <c r="F40" s="11">
         <f>IF(LEN(detail!Z20)&lt;1,"",detail!Z20)</f>
         <v/>
       </c>
-      <c r="G40" s="26">
+      <c r="G40" s="27">
         <f>IF(LEN(detail!W20)&lt;1,"",detail!W20)</f>
         <v/>
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="24">
+      <c r="B41" s="25">
         <f>IF(LEN(detail!I21)&lt;1,"",detail!I21)</f>
         <v/>
       </c>
-      <c r="C41" s="25" t="n"/>
-      <c r="D41" s="26">
+      <c r="C41" s="26" t="n"/>
+      <c r="D41" s="27">
         <f>IF(LEN(detail!P21)&lt;1,"",detail!P21) &amp; IF(detail!K21=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E41" s="25" t="n"/>
+      <c r="E41" s="26" t="n"/>
       <c r="F41" s="11">
         <f>IF(LEN(detail!Z21)&lt;1,"",detail!Z21)</f>
         <v/>
       </c>
-      <c r="G41" s="26">
+      <c r="G41" s="27">
         <f>IF(LEN(detail!W21)&lt;1,"",detail!W21)</f>
         <v/>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="24">
+      <c r="B42" s="25">
         <f>IF(LEN(detail!I22)&lt;1,"",detail!I22)</f>
         <v/>
       </c>
-      <c r="C42" s="25" t="n"/>
-      <c r="D42" s="26">
+      <c r="C42" s="26" t="n"/>
+      <c r="D42" s="27">
         <f>IF(LEN(detail!P22)&lt;1,"",detail!P22) &amp; IF(detail!K22=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E42" s="25" t="n"/>
+      <c r="E42" s="26" t="n"/>
       <c r="F42" s="11">
         <f>IF(LEN(detail!Z22)&lt;1,"",detail!Z22)</f>
         <v/>
       </c>
-      <c r="G42" s="26">
+      <c r="G42" s="27">
         <f>IF(LEN(detail!W22)&lt;1,"",detail!W22)</f>
         <v/>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="24">
+      <c r="B43" s="25">
         <f>IF(LEN(detail!I23)&lt;1,"",detail!I23)</f>
         <v/>
       </c>
-      <c r="C43" s="25" t="n"/>
-      <c r="D43" s="26">
+      <c r="C43" s="26" t="n"/>
+      <c r="D43" s="27">
         <f>IF(LEN(detail!P23)&lt;1,"",detail!P23) &amp; IF(detail!K23=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E43" s="25" t="n"/>
+      <c r="E43" s="26" t="n"/>
       <c r="F43" s="11">
         <f>IF(LEN(detail!Z23)&lt;1,"",detail!Z23)</f>
         <v/>
       </c>
-      <c r="G43" s="26">
+      <c r="G43" s="27">
         <f>IF(LEN(detail!W23)&lt;1,"",detail!W23)</f>
         <v/>
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="24">
+      <c r="B44" s="25">
         <f>IF(LEN(detail!I24)&lt;1,"",detail!I24)</f>
         <v/>
       </c>
-      <c r="C44" s="25" t="n"/>
-      <c r="D44" s="26">
+      <c r="C44" s="26" t="n"/>
+      <c r="D44" s="27">
         <f>IF(LEN(detail!P24)&lt;1,"",detail!P24) &amp; IF(detail!K24=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E44" s="25" t="n"/>
+      <c r="E44" s="26" t="n"/>
       <c r="F44" s="11">
         <f>IF(LEN(detail!Z24)&lt;1,"",detail!Z24)</f>
         <v/>
       </c>
-      <c r="G44" s="26">
+      <c r="G44" s="27">
         <f>IF(LEN(detail!W24)&lt;1,"",detail!W24)</f>
         <v/>
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="24">
+      <c r="B45" s="25">
         <f>IF(LEN(detail!I25)&lt;1,"",detail!I25)</f>
         <v/>
       </c>
-      <c r="C45" s="25" t="n"/>
-      <c r="D45" s="26">
+      <c r="C45" s="26" t="n"/>
+      <c r="D45" s="27">
         <f>IF(LEN(detail!P25)&lt;1,"",detail!P25) &amp; IF(detail!K25=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E45" s="25" t="n"/>
+      <c r="E45" s="26" t="n"/>
       <c r="F45" s="11">
         <f>IF(LEN(detail!Z25)&lt;1,"",detail!Z25)</f>
         <v/>
       </c>
-      <c r="G45" s="26">
+      <c r="G45" s="27">
         <f>IF(LEN(detail!W25)&lt;1,"",detail!W25)</f>
         <v/>
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="24">
+      <c r="B46" s="25">
         <f>IF(LEN(detail!I26)&lt;1,"",detail!I26)</f>
         <v/>
       </c>
-      <c r="C46" s="25" t="n"/>
-      <c r="D46" s="26">
+      <c r="C46" s="26" t="n"/>
+      <c r="D46" s="27">
         <f>IF(LEN(detail!P26)&lt;1,"",detail!P26) &amp; IF(detail!K26=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E46" s="25" t="n"/>
+      <c r="E46" s="26" t="n"/>
       <c r="F46" s="11">
         <f>IF(LEN(detail!Z26)&lt;1,"",detail!Z26)</f>
         <v/>
       </c>
-      <c r="G46" s="26">
+      <c r="G46" s="27">
         <f>IF(LEN(detail!W26)&lt;1,"",detail!W26)</f>
         <v/>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="24">
+      <c r="B47" s="25">
         <f>IF(LEN(detail!I27)&lt;1,"",detail!I27)</f>
         <v/>
       </c>
-      <c r="C47" s="25" t="n"/>
-      <c r="D47" s="26">
+      <c r="C47" s="26" t="n"/>
+      <c r="D47" s="27">
         <f>IF(LEN(detail!P27)&lt;1,"",detail!P27) &amp; IF(detail!K27=1, "*", "")</f>
         <v/>
       </c>
-      <c r="E47" s="25" t="n"/>
+      <c r="E47" s="26" t="n"/>
       <c r="F47" s="11">
         <f>IF(LEN(detail!Z27)&lt;1,"",detail!Z27)</f>
         <v/>
       </c>
-      <c r="G47" s="26">
+      <c r="G47" s="27">
         <f>IF(LEN(detail!W27)&lt;1,"",detail!W27)</f>
         <v/>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="24">
-        <f>IF(LEN(detail!I28)&lt;1,"",detail!I28)</f>
-        <v/>
-      </c>
-      <c r="C48" s="25" t="n"/>
-      <c r="D48" s="26">
-        <f>IF(LEN(detail!P28)&lt;1,"",detail!P28) &amp; IF(detail!K28=1, "*", "")</f>
-        <v/>
-      </c>
-      <c r="E48" s="25" t="n"/>
-      <c r="F48" s="11">
-        <f>IF(LEN(detail!Z28)&lt;1,"",detail!Z28)</f>
-        <v/>
-      </c>
-      <c r="G48" s="26">
-        <f>IF(LEN(detail!W28)&lt;1,"",detail!W28)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" s="1" t="inlineStr">
+      <c r="B48" s="1" t="inlineStr">
         <is>
           <t>An * denotes a targeted payout</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="67">
+  <mergeCells count="65">
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="E9:G9"/>
     <mergeCell ref="D46:E46"/>
-    <mergeCell ref="E9:G9"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="B31:C31"/>
@@ -1822,7 +1807,6 @@
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B48:C48"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B42:C42"/>
@@ -1830,7 +1814,6 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D48:E48"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B38:C38"/>
@@ -1852,11 +1835,11 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="D42:E42"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D42:E42"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D23:E23"/>
@@ -1869,7 +1852,7 @@
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D35:E35"/>
   </mergeCells>
-  <conditionalFormatting sqref="B22:B48 D22:D48 F22:G48">
+  <conditionalFormatting sqref="B22:B47 D22:D47 F22:G47">
     <cfRule type="containsErrors" priority="1" dxfId="0">
       <formula>ISERROR(B22)</formula>
     </cfRule>
@@ -1895,42 +1878,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="inlineStr">
+      <c r="A1" s="45" t="inlineStr">
         <is>
           <t>YYYYMM</t>
         </is>
       </c>
-      <c r="B1" s="44" t="inlineStr">
+      <c r="B1" s="45" t="inlineStr">
         <is>
           <t>EID</t>
         </is>
       </c>
-      <c r="C1" s="44" t="inlineStr">
+      <c r="C1" s="45" t="inlineStr">
         <is>
           <t>YYYYQQ</t>
         </is>
       </c>
-      <c r="D1" s="44" t="inlineStr">
+      <c r="D1" s="45" t="inlineStr">
         <is>
           <t>ROLE</t>
         </is>
       </c>
-      <c r="E1" s="44" t="inlineStr">
+      <c r="E1" s="45" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="F1" s="44" t="inlineStr">
+      <c r="F1" s="45" t="inlineStr">
         <is>
           <t>VALUE</t>
         </is>
       </c>
-      <c r="G1" s="44" t="inlineStr">
+      <c r="G1" s="45" t="inlineStr">
         <is>
           <t>CATEGORY</t>
         </is>
       </c>
-      <c r="H1" s="44" t="inlineStr">
+      <c r="H1" s="45" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
@@ -1939,17 +1922,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1963,7 +1946,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>28473</v>
+        <v>1523.28</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -1974,17 +1957,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1998,7 +1981,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -2009,17 +1992,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2033,7 +2016,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>969000</v>
+        <v>644000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2044,17 +2027,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2068,7 +2051,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>12023.03</v>
+        <v>1523.28</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2079,17 +2062,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2103,7 +2086,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -2114,17 +2097,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2138,7 +2121,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -2149,17 +2132,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -2173,7 +2156,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2292.02</v>
+        <v>1523.28</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -2184,17 +2167,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2208,7 +2191,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5092.02</v>
+        <v>1523.28</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -2219,17 +2202,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2243,7 +2226,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -2254,17 +2237,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2278,7 +2261,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>5083000</v>
+        <v>644000</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -2289,17 +2272,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -2324,17 +2307,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -2348,7 +2331,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>5242.02</v>
+        <v>1523.28</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -2367,10 +2350,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -2385,6 +2368,11 @@
           <t>Name:</t>
         </is>
       </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Zilma Colon</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2394,7 +2382,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
     </row>
@@ -2404,6 +2392,11 @@
           <t>RM:</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kryan@cvrx.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2411,6 +2404,11 @@
           <t>Territory:</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FLORIDA (COLON)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2430,6 +2428,9 @@
           <t>Base Bonus:</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>30000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2439,8 +2440,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>June</t>
-        </is>
+          <t>July</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Quota:</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12683164</v>
       </c>
     </row>
     <row r="21" ht="15.95" customHeight="1"/>
@@ -2458,7 +2469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC24"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2467,147 +2478,147 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="44" t="inlineStr">
+      <c r="A1" s="45" t="inlineStr">
         <is>
           <t>SALES_CREDIT_FCE_EMAIL</t>
         </is>
       </c>
-      <c r="B1" s="44" t="inlineStr">
+      <c r="B1" s="45" t="inlineStr">
         <is>
           <t>NAME_REP</t>
         </is>
       </c>
-      <c r="C1" s="44" t="inlineStr">
+      <c r="C1" s="45" t="inlineStr">
         <is>
           <t>SALES_CREDIT_REP_EMAIL</t>
         </is>
       </c>
-      <c r="D1" s="44" t="inlineStr">
+      <c r="D1" s="45" t="inlineStr">
         <is>
           <t>ROLE</t>
         </is>
       </c>
-      <c r="E1" s="44" t="inlineStr">
+      <c r="E1" s="45" t="inlineStr">
         <is>
           <t>DOH</t>
         </is>
       </c>
-      <c r="F1" s="44" t="inlineStr">
+      <c r="F1" s="45" t="inlineStr">
         <is>
           <t>CLOSEDATE</t>
         </is>
       </c>
-      <c r="G1" s="44" t="inlineStr">
+      <c r="G1" s="45" t="inlineStr">
         <is>
           <t>REGION</t>
         </is>
       </c>
-      <c r="H1" s="44" t="inlineStr">
+      <c r="H1" s="45" t="inlineStr">
         <is>
           <t>REGION_ID</t>
         </is>
       </c>
-      <c r="I1" s="44" t="inlineStr">
+      <c r="I1" s="45" t="inlineStr">
         <is>
           <t>ACCOUNT</t>
         </is>
       </c>
-      <c r="J1" s="44" t="inlineStr">
+      <c r="J1" s="45" t="inlineStr">
         <is>
           <t>PHYSICIAN</t>
         </is>
       </c>
-      <c r="K1" s="44" t="inlineStr">
+      <c r="K1" s="45" t="inlineStr">
         <is>
           <t>isTarget?</t>
         </is>
       </c>
-      <c r="L1" s="44" t="inlineStr">
+      <c r="L1" s="45" t="inlineStr">
         <is>
           <t>PO_%</t>
         </is>
       </c>
-      <c r="M1" s="44" t="inlineStr">
+      <c r="M1" s="45" t="inlineStr">
         <is>
           <t>PO_PER</t>
         </is>
       </c>
-      <c r="N1" s="44" t="inlineStr">
+      <c r="N1" s="45" t="inlineStr">
         <is>
           <t>CPAS_SPIFF_DEDUCTION</t>
         </is>
       </c>
-      <c r="O1" s="44" t="inlineStr">
+      <c r="O1" s="45" t="inlineStr">
         <is>
           <t>TGT_PO</t>
         </is>
       </c>
-      <c r="P1" s="44" t="inlineStr">
+      <c r="P1" s="45" t="inlineStr">
         <is>
           <t>OPP_NAME</t>
         </is>
       </c>
-      <c r="Q1" s="44" t="inlineStr">
+      <c r="Q1" s="45" t="inlineStr">
         <is>
           <t>OPP_ID</t>
         </is>
       </c>
-      <c r="R1" s="44" t="inlineStr">
+      <c r="R1" s="45" t="inlineStr">
         <is>
           <t>IPG</t>
         </is>
       </c>
-      <c r="S1" s="44" t="inlineStr">
+      <c r="S1" s="45" t="inlineStr">
         <is>
           <t>CLOSE_YYYYMM</t>
         </is>
       </c>
-      <c r="T1" s="44" t="inlineStr">
+      <c r="T1" s="45" t="inlineStr">
         <is>
           <t>CLOSE_YYYYQQ</t>
         </is>
       </c>
-      <c r="U1" s="44" t="inlineStr">
+      <c r="U1" s="45" t="inlineStr">
         <is>
           <t>IMPLANTED_YYYYMM</t>
         </is>
       </c>
-      <c r="V1" s="44" t="inlineStr">
+      <c r="V1" s="45" t="inlineStr">
         <is>
           <t>IMPLANTED_YYYYQQ</t>
         </is>
       </c>
-      <c r="W1" s="44" t="inlineStr">
+      <c r="W1" s="45" t="inlineStr">
         <is>
           <t>QTY</t>
         </is>
       </c>
-      <c r="X1" s="44" t="inlineStr">
+      <c r="X1" s="45" t="inlineStr">
         <is>
           <t>SALES_BASE</t>
         </is>
       </c>
-      <c r="Y1" s="44" t="inlineStr">
+      <c r="Y1" s="45" t="inlineStr">
         <is>
           <t>SALES_TGT</t>
         </is>
       </c>
-      <c r="Z1" s="44" t="inlineStr">
+      <c r="Z1" s="45" t="inlineStr">
         <is>
           <t>SALES</t>
         </is>
       </c>
-      <c r="AA1" s="44" t="inlineStr">
+      <c r="AA1" s="45" t="inlineStr">
         <is>
           <t>isComp?</t>
         </is>
       </c>
-      <c r="AB1" s="44" t="inlineStr">
+      <c r="AB1" s="45" t="inlineStr">
         <is>
           <t>TYPE</t>
         </is>
       </c>
-      <c r="AC1" s="44" t="inlineStr">
+      <c r="AC1" s="45" t="inlineStr">
         <is>
           <t>isDUPE?</t>
         </is>
@@ -2616,17 +2627,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jclemmons@cvrx.com</t>
+          <t>mmuratovic@cvrx.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2634,13 +2645,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E2" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-06-04</t>
-        </is>
+      <c r="E2" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F2" s="49" t="n">
+        <v>45484</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -2654,79 +2663,66 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Adventhealth Orlando</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Pujan Patel</t>
-        </is>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
+          <t>Tampa General Hospital</t>
+        </is>
       </c>
       <c r="M2" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>AHOrl 015460</t>
+          <t>TPA01 020022</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>0064u00001ILN76AAH</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>2104012387</t>
+          <t>006UY00000A34cPYAR</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X2" t="n">
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="Y2" t="n">
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>28000</v>
+        <v>56000</v>
       </c>
       <c r="AA2" t="n">
         <v>1</v>
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>ACCT</t>
+          <t>REGION_HF</t>
         </is>
       </c>
       <c r="AC2" t="n">
@@ -2736,12 +2732,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2754,13 +2750,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E3" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-06-05</t>
-        </is>
+      <c r="E3" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F3" s="49" t="n">
+        <v>45490</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -2793,37 +2787,37 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>CRX137 019474</t>
+          <t>CRX137 020230</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>006UY0000096nYjYAI</t>
+          <t>006UY00000AQ9LFYA1</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>2104012334</t>
+          <t>2104012417</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W3" t="n">
@@ -2853,12 +2847,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2871,13 +2865,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E4" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-06-05</t>
-        </is>
+      <c r="E4" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F4" s="49" t="n">
+        <v>45490</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -2891,7 +2883,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Tampa General Hospital</t>
+          <t>Adventhealth Tampa</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Natasha Mehta</t>
         </is>
       </c>
       <c r="M4" t="n">
@@ -2905,45 +2902,50 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>TPA01 019555</t>
+          <t>CRX846 020281</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>006UY000009FmS9YAK</t>
+          <t>006UY00000AX8U6YAL</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>2104012312</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W4" t="n">
         <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>35000</v>
+        <v>28000</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>35000</v>
+        <v>28000</v>
       </c>
       <c r="AA4" t="n">
         <v>1</v>
@@ -2960,17 +2962,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>aavalos@cvrx.com</t>
+          <t>jwaguespack@cvrx.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2978,13 +2980,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E5" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-06-07</t>
-        </is>
+      <c r="E5" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F5" s="49" t="n">
+        <v>45491</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -2998,7 +2998,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Bethesda Hospital West</t>
+          <t>Christus Health Shreveport - Bossier</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Elizabeth Willis</t>
         </is>
       </c>
       <c r="M5" t="n">
@@ -3012,45 +3017,50 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>BHW 019336</t>
+          <t>CRX137 020231</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>006UY000008nLmgYAE</t>
+          <t>006UY00000AQ9l3YAD</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2104012415</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X5" t="n">
-        <v>63000</v>
+        <v>35000</v>
       </c>
       <c r="Y5" t="n">
         <v>0</v>
       </c>
       <c r="Z5" t="n">
-        <v>63000</v>
+        <v>35000</v>
       </c>
       <c r="AA5" t="n">
         <v>1</v>
@@ -3067,17 +3077,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>aavalos@cvrx.com</t>
+          <t>ataylor@cvrx.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3085,13 +3095,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E6" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-06-07</t>
-        </is>
+      <c r="E6" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F6" s="49" t="n">
+        <v>45492</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -3105,7 +3113,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Bethesda Hospital East</t>
+          <t>Adventhealth Daytona Beach</t>
         </is>
       </c>
       <c r="M6" t="n">
@@ -3119,45 +3127,45 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>BHE01 019514</t>
+          <t>AHDB 020440</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>006UY00000991anYAA</t>
+          <t>006UY00000Au5DlYAJ</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W6" t="n">
         <v>1</v>
       </c>
       <c r="X6" t="n">
-        <v>31500</v>
+        <v>28000</v>
       </c>
       <c r="Y6" t="n">
         <v>0</v>
       </c>
       <c r="Z6" t="n">
-        <v>31500</v>
+        <v>28000</v>
       </c>
       <c r="AA6" t="n">
         <v>1</v>
@@ -3174,17 +3182,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>mwhitney@cvrx.com</t>
+          <t>tmcdonald@cvrx.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3192,13 +3200,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E7" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-06-07</t>
-        </is>
+      <c r="E7" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F7" s="49" t="n">
+        <v>45495</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -3212,7 +3218,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Tallahassee Memorial Healthcare</t>
+          <t>Sarasota Memorial Health Care System</t>
         </is>
       </c>
       <c r="M7" t="n">
@@ -3226,45 +3232,45 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>CRX654 019666</t>
+          <t>SMH 019939</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>006UY000009Q9VjYAK</t>
+          <t>006UY000009tFfaYAE</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W7" t="n">
         <v>3</v>
       </c>
       <c r="X7" t="n">
-        <v>99000</v>
+        <v>84000</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>99000</v>
+        <v>84000</v>
       </c>
       <c r="AA7" t="n">
         <v>1</v>
@@ -3281,17 +3287,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>aavalos@cvrx.com</t>
+          <t>jclemmons@cvrx.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3299,13 +3305,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E8" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-06-11</t>
-        </is>
+      <c r="E8" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F8" s="49" t="n">
+        <v>45496</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -3319,12 +3323,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Jfk Medical Center</t>
+          <t>Adventhealth Celebration</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Israel Henriquez</t>
+          <t>Glenn Dym</t>
         </is>
       </c>
       <c r="M8" t="n">
@@ -3338,37 +3342,37 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>JFKMC 017928</t>
+          <t>AHCE 019645</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>006UY000005oVFSYA2</t>
+          <t>006UY000009P6t4YAC</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>2104012481</t>
+          <t>2104012571</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W8" t="n">
@@ -3398,12 +3402,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3416,13 +3420,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E9" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-06-12</t>
-        </is>
+      <c r="E9" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F9" s="49" t="n">
+        <v>45496</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -3441,64 +3443,61 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Tess Espiritu</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
+          <t>Deepti Bhandare</t>
+        </is>
       </c>
       <c r="M9" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>AHCE 016731</t>
+          <t>AHCE 017338</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>006UY0000033GEbYAM</t>
+          <t>006UY000004dwxwYAA</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>2104012442</t>
+          <t>2104012572</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W9" t="n">
         <v>1</v>
       </c>
       <c r="X9" t="n">
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="Y9" t="n">
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="Z9" t="n">
         <v>28000</v>
@@ -3508,7 +3507,7 @@
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>ACCT</t>
+          <t>REGION_HF</t>
         </is>
       </c>
       <c r="AC9" t="n">
@@ -3518,17 +3517,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>jclemmons@cvrx.com</t>
+          <t>mmuratovic@cvrx.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3536,13 +3535,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E10" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2024-06-12</t>
-        </is>
+      <c r="E10" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F10" s="49" t="n">
+        <v>45497</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -3556,69 +3553,66 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Adventhealth Orlando</t>
+          <t>Adventhealth Tampa</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Pujan Patel</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>1</v>
+          <t>Hector Fontanet</t>
+        </is>
       </c>
       <c r="M10" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>AHOrl 017099</t>
+          <t>CRX846 020222</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>006UY0000045VbyYAE</t>
+          <t>006UY00000ANTpxYAH</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>2104012441</t>
+          <t>2104012010</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W10" t="n">
         <v>1</v>
       </c>
       <c r="X10" t="n">
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="Y10" t="n">
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="Z10" t="n">
         <v>28000</v>
@@ -3628,7 +3622,7 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>ACCT</t>
+          <t>REGION_HF</t>
         </is>
       </c>
       <c r="AC10" t="n">
@@ -3638,17 +3632,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>jclemmons@cvrx.com</t>
+          <t>aavalos@cvrx.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3656,13 +3650,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E11" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2024-06-12</t>
-        </is>
+      <c r="E11" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F11" s="49" t="n">
+        <v>45497</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -3676,7 +3668,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Adventhealth Orlando</t>
+          <t>Jfk Medical Center</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Sajid Mirza</t>
         </is>
       </c>
       <c r="M11" t="n">
@@ -3690,37 +3687,37 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>AHOrl 019532</t>
+          <t>JFKMC 020515</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>006UY000009DaWkYAK</t>
+          <t>006UY00000B2rczYAB</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>2104012468</t>
+          <t>2104012482</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W11" t="n">
@@ -3750,17 +3747,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>jwaguespack@cvrx.com</t>
+          <t>mwhitney@cvrx.com</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3768,13 +3765,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E12" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2024-06-13</t>
-        </is>
+      <c r="E12" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F12" s="49" t="n">
+        <v>45497</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -3788,12 +3783,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Christus Health Shreveport - Bossier</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Elizabeth Willis</t>
+          <t>Tallahassee Memorial Healthcare</t>
         </is>
       </c>
       <c r="M12" t="n">
@@ -3807,50 +3797,45 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>CRX137 016858</t>
+          <t>CRX654 020523</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>006UY000003WBt9YAG</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>2104012416</t>
+          <t>006UY00000B4YUcYAN</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X12" t="n">
-        <v>35000</v>
+        <v>94500</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
       </c>
       <c r="Z12" t="n">
-        <v>35000</v>
+        <v>94500</v>
       </c>
       <c r="AA12" t="n">
         <v>1</v>
@@ -3867,17 +3852,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>tmcdonald@cvrx.com</t>
+          <t>jclemmons@cvrx.com</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3885,13 +3870,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E13" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2024-06-17</t>
-        </is>
+      <c r="E13" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F13" s="49" t="n">
+        <v>45502</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -3905,12 +3888,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Lee Memorial Hs- Cape Coral Hosp</t>
+          <t>Adventhealth Celebration</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Bill Richardson</t>
+          <t>Pradip Jamnadas</t>
         </is>
       </c>
       <c r="M13" t="n">
@@ -3924,50 +3907,50 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>CCH 018187</t>
+          <t>AHCE 018274</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>006UY000006RhS6YAK</t>
+          <t>006UY000006kfKrYAI</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>2104012393</t>
+          <t>2104012473</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W13" t="n">
         <v>1</v>
       </c>
       <c r="X13" t="n">
-        <v>31500</v>
+        <v>28000</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
       </c>
       <c r="Z13" t="n">
-        <v>31500</v>
+        <v>28000</v>
       </c>
       <c r="AA13" t="n">
         <v>1</v>
@@ -3984,17 +3967,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ralvarez@cvrx.com</t>
+          <t>zcolon@cvrx.com</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Raul Alvarez</t>
+          <t>Zilma Colon</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>jclemmons@cvrx.com</t>
+          <t>jdray@cvrx.com</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4002,13 +3985,11 @@
           <t>FCE</t>
         </is>
       </c>
-      <c r="E14" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2024-06-18</t>
-        </is>
+      <c r="E14" s="48" t="n">
+        <v>45467</v>
+      </c>
+      <c r="F14" s="49" t="n">
+        <v>45504</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -4022,1191 +4003,69 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Adventhealth Orlando</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>1</v>
+          <t>Uf Health Leesburg Hospital</t>
+        </is>
       </c>
       <c r="M14" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>AHOrl 019783</t>
+          <t>CRX680 017279</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>006UY000009dnenYAA</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>2104012440</t>
+          <t>006UY000004XiKvYAK</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>2024_06</t>
+          <t>2024_07</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>2024_Q2</t>
+          <t>2024_Q3</t>
         </is>
       </c>
       <c r="W14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X14" t="n">
-        <v>0</v>
+        <v>84000</v>
       </c>
       <c r="Y14" t="n">
-        <v>28000</v>
+        <v>0</v>
       </c>
       <c r="Z14" t="n">
-        <v>28000</v>
+        <v>84000</v>
       </c>
       <c r="AA14" t="n">
         <v>1</v>
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>ACCT</t>
+          <t>REGION_HF</t>
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>jclemmons@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E15" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2024-06-19</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Adventhealth Orlando</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Naveen Bellam</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" t="n">
-        <v>400</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>400</v>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>AHOrl 015977</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>0064u00001IyFOtAAN</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>2104012469</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W15" t="n">
-        <v>1</v>
-      </c>
-      <c r="X15" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>28000</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>28000</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t>ACCT</t>
-        </is>
-      </c>
-      <c r="AC15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>jwaguespack@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E16" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2024-06-20</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Willis Knighton Medical Center, Inc</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>CRX953 019636</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>006UY000009MsuDYAS</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W16" t="n">
-        <v>3</v>
-      </c>
-      <c r="X16" t="n">
-        <v>99000</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>99000</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>jclemmons@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E17" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2024-06-21</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Adventhealth Orlando</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Prabhakara Kunamneni</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" t="n">
-        <v>400</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
-        <v>400</v>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>AHOrl 014701</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>0064u00001HqgGyAAJ</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>2104012471</t>
-        </is>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W17" t="n">
-        <v>1</v>
-      </c>
-      <c r="X17" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>28000</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>28000</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t>ACCT</t>
-        </is>
-      </c>
-      <c r="AC17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>aavalos@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E18" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2024-06-26</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Westside Regional Medical Center</t>
-        </is>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>WRMC724 019307</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>006UY000008k36LYAQ</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W18" t="n">
-        <v>3</v>
-      </c>
-      <c r="X18" t="n">
-        <v>84000</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>84000</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB18" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>mwhitney@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E19" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2024-06-27</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Tallahassee Memorial Healthcare</t>
-        </is>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>CRX654 019526</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>006UY000009CbHxYAK</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T19" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V19" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W19" t="n">
-        <v>3</v>
-      </c>
-      <c r="X19" t="n">
-        <v>99000</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>99000</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>jclemmons@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E20" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>2024-06-28</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Adventhealth Orlando</t>
-        </is>
-      </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
-      <c r="M20" t="n">
-        <v>400</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>400</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>AHOrl 019946</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>006UY000009torpYAA</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>2104012573</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T20" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W20" t="n">
-        <v>1</v>
-      </c>
-      <c r="X20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>28000</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>28000</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>ACCT</t>
-        </is>
-      </c>
-      <c r="AC20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>jclemmons@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E21" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>2024-06-28</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Holmes Regional Medical Center</t>
-        </is>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>CRX266 020077</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>006UY00000A9BJRYA3</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V21" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W21" t="n">
-        <v>1</v>
-      </c>
-      <c r="X21" t="n">
-        <v>31500</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>31500</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB21" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>mmuratovic@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E22" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>2024-06-28</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Adventhealth Zephyrhills</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Natasha Mehta</t>
-        </is>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>CRX832 017986</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>006UY000005zfRbYAI</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>2104012311</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T22" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W22" t="n">
-        <v>1</v>
-      </c>
-      <c r="X22" t="n">
-        <v>28000</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>28000</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB22" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>mmuratovic@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E23" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>2024-06-30</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Tampa General Hospital</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>TPA01 020114</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>006UY00000ABgJ8YAL</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T23" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V23" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W23" t="n">
-        <v>0</v>
-      </c>
-      <c r="X23" t="n">
-        <v>14000</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>14000</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB23" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>ralvarez@cvrx.com</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Raul Alvarez</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>dabesamis@cvrx.com</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>FCE</t>
-        </is>
-      </c>
-      <c r="E24" s="46" t="n">
-        <v>43983</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>2024-06-30</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>RE_06</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Holy Cross Health</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>FLL01 020034</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>006UY00000A4MVfYAN</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="T24" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>2024_06</t>
-        </is>
-      </c>
-      <c r="V24" t="inlineStr">
-        <is>
-          <t>2024_Q2</t>
-        </is>
-      </c>
-      <c r="W24" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" t="n">
-        <v>3500</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>3500</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB24" t="inlineStr">
-        <is>
-          <t>REGION_HF</t>
-        </is>
-      </c>
-      <c r="AC24" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>